<commit_message>
refactor: update dataframe to file cases
</commit_message>
<xml_diff>
--- a/1221_pandas/stu.xlsx
+++ b/1221_pandas/stu.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,72 +434,50 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>姓名</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>语文</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>数学</t>
+          <t>姓名,语文,数学</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
-          <t>小明</t>
+          <t>小明,90,92</t>
         </is>
-      </c>
-      <c r="B2" t="n">
-        <v>90</v>
-      </c>
-      <c r="C2" t="n">
-        <v>92</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
-          <t>小红</t>
+          <t>小红,98,87</t>
         </is>
-      </c>
-      <c r="B3" t="n">
-        <v>98</v>
-      </c>
-      <c r="C3" t="n">
-        <v>87</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
-          <t>小刚</t>
+          <t>小刚,87,90</t>
         </is>
-      </c>
-      <c r="B4" t="n">
-        <v>87</v>
-      </c>
-      <c r="C4" t="n">
-        <v>90</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
-          <t>小丽</t>
+          <t>小丽,90,98</t>
         </is>
-      </c>
-      <c r="B5" t="n">
-        <v>90</v>
-      </c>
-      <c r="C5" t="n">
-        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>